<commit_message>
第12次提交： samples/s1_demo.py importdata.py整合excel实战 common/requests_utils.py 添加异常处理
</commit_message>
<xml_diff>
--- a/samples/data/test_case.xlsx
+++ b/samples/data/test_case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23117"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python\Scripts\API_TEST_FRAME\samples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46A6B77-B9F1-4E91-AFBF-2DE9D0166542}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8443821A-10A8-4C8E-9011-5298160DAEB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="135" yWindow="195" windowWidth="23970" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>json键是否存在</t>
   </si>
   <si>
-    <t>access_token,expires_in</t>
-  </si>
-  <si>
     <t>case02</t>
   </si>
   <si>
@@ -165,6 +162,10 @@
   </si>
   <si>
     <t>/cgi-bin/tags/delete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>access_token1,expires_in</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -232,10 +233,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -516,7 +517,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -612,19 +613,19 @@
       <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
-        <v>24</v>
+      <c r="N2" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -642,61 +643,61 @@
         <v>21</v>
       </c>
       <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>29</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
       <c r="N3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
       <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>35</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>36</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>37</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
@@ -715,51 +716,51 @@
         <v>21</v>
       </c>
       <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
         <v>28</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>29</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>30</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>31</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
         <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
       </c>
       <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" t="s">
         <v>44</v>
-      </c>
-      <c r="N6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="25.5" x14ac:dyDescent="0.15">

</xml_diff>